<commit_message>
- prevent printing of crypt text
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_expressions_more.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_expressions_more.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" tabRatio="500"/>
+    <workbookView windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -72,18 +72,33 @@
   <si>
     <t>nexial.openResult</t>
   </si>
+  <si>
+    <t>nexial.browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>nexial.browser.incognito</t>
+  </si>
+  <si>
+    <t>nexial.browser.userData</t>
+  </si>
+  <si>
+    <t>/Users/mliu/Library/Application Support/Google/Chrome/Default</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -114,6 +129,44 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -122,8 +175,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -131,22 +206,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,7 +222,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -175,65 +236,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +250,35 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -258,25 +289,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,157 +457,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,6 +498,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -482,11 +522,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,197 +595,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -741,54 +778,56 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="60% - Accent4" xfId="10" builtinId="44"/>
-    <cellStyle name="40% - Accent3" xfId="11" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="12" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="13" builtinId="35"/>
-    <cellStyle name="Title" xfId="14" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="15" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="17" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="18" builtinId="19"/>
-    <cellStyle name="Input" xfId="19" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="20" builtinId="40"/>
-    <cellStyle name="Good" xfId="21" builtinId="26"/>
-    <cellStyle name="Output" xfId="22" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="23" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="24" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="25" builtinId="24"/>
-    <cellStyle name="Total" xfId="26" builtinId="25"/>
-    <cellStyle name="Bad" xfId="27" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="29" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="30" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="31" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="33" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="34" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="35" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="37" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="38" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="39" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="40" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="42" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="43" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="44" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="45" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="46" builtinId="52"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1152,15 +1191,15 @@
   <dimension ref="A1:AAA200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.8533333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.2866666666667" style="2" customWidth="1"/>
-    <col min="3" max="52" width="21.2866666666667" style="3" customWidth="1"/>
-    <col min="53" max="16384" width="10.7133333333333" style="3"/>
+    <col min="1" max="1" width="34.8541666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.2847222222222" style="2" customWidth="1"/>
+    <col min="3" max="52" width="21.2847222222222" style="3" customWidth="1"/>
+    <col min="53" max="16384" width="10.7152777777778" style="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="23" customHeight="1" spans="1:703">
@@ -1234,17 +1273,32 @@
       <c r="AAA7" s="7"/>
     </row>
     <row r="8" ht="23" customHeight="1" spans="1:703">
-      <c r="A8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="HA8" s="6"/>
       <c r="AAA8" s="7"/>
     </row>
     <row r="9" ht="23" customHeight="1" spans="1:703">
-      <c r="A9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="HA9" s="6"/>
       <c r="AAA9" s="7"/>
     </row>
     <row r="10" ht="23" customHeight="1" spans="1:703">
-      <c r="A10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="HA10" s="6"/>
       <c r="AAA10" s="7"/>
     </row>

</xml_diff>